<commit_message>
support download file to pointed path
</commit_message>
<xml_diff>
--- a/UI/getdata/TestData.xlsx
+++ b/UI/getdata/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20357"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79C4906-9698-4F27-B346-401A8D0E7239}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD588DA9-2CAF-43DE-AF5E-AC5CFFF65E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="3" r:id="rId1"/>
@@ -512,15 +512,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Adjustment-Dispositions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>customers</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Read Only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjustment - Dispositions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1041,7 +1041,7 @@
         <v>72</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="2" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>114</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="3" spans="1:4" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>114</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="4" spans="1:4" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>114</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="5" spans="1:4" ht="252" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>121</v>
@@ -1573,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0BEE8E-9587-4F3A-B317-A4C90C197E77}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1699,7 +1699,7 @@
         <v>106</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
update the database's pwd
</commit_message>
<xml_diff>
--- a/UI/getdata/TestData.xlsx
+++ b/UI/getdata/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="297">
   <si>
     <t>fieldName</t>
   </si>
@@ -122,123 +122,129 @@
     <t>vewLookupIdentifierNameWithoutBan</t>
   </si>
   <si>
+    <t>interestClass</t>
+  </si>
+  <si>
+    <t>ltblInterestClass</t>
+  </si>
+  <si>
+    <t>varInterestClass</t>
+  </si>
+  <si>
+    <t>interestStatus</t>
+  </si>
+  <si>
+    <t>ltblInterestStatus</t>
+  </si>
+  <si>
+    <t>varInterestStatus</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>ltblCountyToRRCDistrictNumber</t>
+  </si>
+  <si>
+    <t>varCountyName</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Utilization Class</t>
+  </si>
+  <si>
+    <t>ltblUtilizationClass</t>
+  </si>
+  <si>
+    <t>varUtilizationClass</t>
+  </si>
+  <si>
+    <t>Utilization Type</t>
+  </si>
+  <si>
+    <t>ltblUtilizationType</t>
+  </si>
+  <si>
+    <t>varUtilizationType</t>
+  </si>
+  <si>
+    <t>Land Comment Class</t>
+  </si>
+  <si>
+    <t>ltblLandCommentClass</t>
+  </si>
+  <si>
+    <t>varLandCommentClass</t>
+  </si>
+  <si>
+    <t>Multi Tract Sale Indicator</t>
+  </si>
+  <si>
+    <t>ltblMultiTractSaleIndicator</t>
+  </si>
+  <si>
+    <t>varMultiTractSaleIndicator</t>
+  </si>
+  <si>
+    <t>Easement Disclaimer</t>
+  </si>
+  <si>
+    <t>varEasementDisclaimer</t>
+  </si>
+  <si>
+    <t>Reservation Easement</t>
+  </si>
+  <si>
+    <t>ltblReservationEasementIndicator</t>
+  </si>
+  <si>
+    <t>varReservationEasementIndicator</t>
+  </si>
+  <si>
+    <t>Reservations</t>
+  </si>
+  <si>
+    <t>ltblReservations</t>
+  </si>
+  <si>
+    <t>varReservations</t>
+  </si>
+  <si>
+    <t>Terms Offered</t>
+  </si>
+  <si>
+    <t>ltblTermsOffered</t>
+  </si>
+  <si>
+    <t>varTermsOffered</t>
+  </si>
+  <si>
+    <t>Direction from Seat</t>
+  </si>
+  <si>
+    <t>ltblDirectionFromCountySeat</t>
+  </si>
+  <si>
+    <t>varDirectionFromCountySeat</t>
+  </si>
+  <si>
+    <t>Deviation from Seat</t>
+  </si>
+  <si>
+    <t>ltblDeviationFromCountySeat</t>
+  </si>
+  <si>
+    <t>varDeviationFromCountySeat</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>VewLookupCity</t>
   </si>
   <si>
-    <t>interestClass</t>
-  </si>
-  <si>
-    <t>ltblInterestClass</t>
-  </si>
-  <si>
-    <t>varInterestClass</t>
-  </si>
-  <si>
-    <t>interestStatus</t>
-  </si>
-  <si>
-    <t>ltblInterestStatus</t>
-  </si>
-  <si>
-    <t>varInterestStatus</t>
-  </si>
-  <si>
-    <t>county</t>
-  </si>
-  <si>
-    <t>ltblCountyToRRCDistrictNumber</t>
-  </si>
-  <si>
-    <t>varCountyName</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>Utilization Class</t>
-  </si>
-  <si>
-    <t>ltblUtilizationClass</t>
-  </si>
-  <si>
-    <t>varUtilizationClass</t>
-  </si>
-  <si>
-    <t>Utilization Type</t>
-  </si>
-  <si>
-    <t>ltblUtilizationType</t>
-  </si>
-  <si>
-    <t>varUtilizationType</t>
-  </si>
-  <si>
-    <t>Land Comment Class</t>
-  </si>
-  <si>
-    <t>ltblLandCommentClass</t>
-  </si>
-  <si>
-    <t>varLandCommentClass</t>
-  </si>
-  <si>
-    <t>Multi Tract Sale Indicator</t>
-  </si>
-  <si>
-    <t>ltblMultiTractSaleIndicator</t>
-  </si>
-  <si>
-    <t>varMultiTractSaleIndicator</t>
-  </si>
-  <si>
-    <t>Reservation Easement</t>
-  </si>
-  <si>
-    <t>ltblReservationEasementIndicator</t>
-  </si>
-  <si>
-    <t>varReservationEasementIndicator</t>
-  </si>
-  <si>
-    <t>Reservations</t>
-  </si>
-  <si>
-    <t>ltblReservations</t>
-  </si>
-  <si>
-    <t>varReservations</t>
-  </si>
-  <si>
-    <t>Terms Offered</t>
-  </si>
-  <si>
-    <t>ltblTermsOffered</t>
-  </si>
-  <si>
-    <t>varTermsOffered</t>
-  </si>
-  <si>
-    <t>Direction from Seat</t>
-  </si>
-  <si>
-    <t>ltblDirectionFromCountySeat</t>
-  </si>
-  <si>
-    <t>varDirectionFromCountySeat</t>
-  </si>
-  <si>
-    <t>Deviation from Seat</t>
-  </si>
-  <si>
-    <t>ltblDeviationFromCountySeat</t>
-  </si>
-  <si>
-    <t>varDeviationFromCountySeat</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>varLandCityName</t>
   </si>
   <si>
@@ -258,6 +264,330 @@
   </si>
   <si>
     <t>varWithinCityIndicator</t>
+  </si>
+  <si>
+    <t>Encumbrance Class</t>
+  </si>
+  <si>
+    <t>ltblLandEncumbranceClass</t>
+  </si>
+  <si>
+    <t>varLandEncumbranceClass</t>
+  </si>
+  <si>
+    <t>Improvement Type</t>
+  </si>
+  <si>
+    <t>ltblImprovementType</t>
+  </si>
+  <si>
+    <t>varImprovementType</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>ltblDispositionAttribute</t>
+  </si>
+  <si>
+    <t>varAttributes</t>
+  </si>
+  <si>
+    <t>Improvements Indicator</t>
+  </si>
+  <si>
+    <t>ltblImprovementsIndicator</t>
+  </si>
+  <si>
+    <t>varImprovementsIndicator</t>
+  </si>
+  <si>
+    <t>Utilities Available Indicator</t>
+  </si>
+  <si>
+    <t>ltblUtilitiesAvailableIndicator</t>
+  </si>
+  <si>
+    <t>varUtilitiesAvailableIndicator</t>
+  </si>
+  <si>
+    <t>Surrounding Use Class</t>
+  </si>
+  <si>
+    <t>ltblSurroundingUseClass</t>
+  </si>
+  <si>
+    <t>varSurroundingUseClass</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>ltblBasefilePrefix</t>
+  </si>
+  <si>
+    <t>varBasefilePrefix</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>ltblBasefileSuffix</t>
+  </si>
+  <si>
+    <t>varBasefileSuffix</t>
+  </si>
+  <si>
+    <t>Acquisition Class</t>
+  </si>
+  <si>
+    <t>ltblAcquisitionClass</t>
+  </si>
+  <si>
+    <t>varAcquisitionClass</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>ltblAcquisitionMethod</t>
+  </si>
+  <si>
+    <t>varAcquisitionMethod</t>
+  </si>
+  <si>
+    <t>County Name</t>
+  </si>
+  <si>
+    <t>Excess Status</t>
+  </si>
+  <si>
+    <t>ltblExcessStatus</t>
+  </si>
+  <si>
+    <t>varExcessStatus</t>
+  </si>
+  <si>
+    <t>Minerals Sold Indicator</t>
+  </si>
+  <si>
+    <t>varMineralsSoldIndicator</t>
+  </si>
+  <si>
+    <t>Water Body</t>
+  </si>
+  <si>
+    <t>ltblWaterbody</t>
+  </si>
+  <si>
+    <t>varWaterBody</t>
+  </si>
+  <si>
+    <t>Relate Class</t>
+  </si>
+  <si>
+    <t>varRelateLandToLandRelateClass</t>
+  </si>
+  <si>
+    <t>Land Type</t>
+  </si>
+  <si>
+    <t>ltblLandType</t>
+  </si>
+  <si>
+    <t>varLandType</t>
+  </si>
+  <si>
+    <t>Ownership Class</t>
+  </si>
+  <si>
+    <t>ltblLandOwnershipClass</t>
+  </si>
+  <si>
+    <t>varLandOwnershipClass</t>
+  </si>
+  <si>
+    <t>Geographic Class</t>
+  </si>
+  <si>
+    <t>ltblLandGeographicClass</t>
+  </si>
+  <si>
+    <t>varLandGeographicClass</t>
+  </si>
+  <si>
+    <t>Land Class</t>
+  </si>
+  <si>
+    <t>ltblLandClass</t>
+  </si>
+  <si>
+    <t>varLandDomainClass</t>
+  </si>
+  <si>
+    <t>Land Status</t>
+  </si>
+  <si>
+    <t>ltblLandStatus</t>
+  </si>
+  <si>
+    <t>varLandStatus</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>ltblAppraisalSource</t>
+  </si>
+  <si>
+    <t>varAppraisalSource</t>
+  </si>
+  <si>
+    <t>Estimated Value Method</t>
+  </si>
+  <si>
+    <t>ltblEstimatedValueMethod</t>
+  </si>
+  <si>
+    <t>varEstimatedValueMethod</t>
+  </si>
+  <si>
+    <t>Utility Type</t>
+  </si>
+  <si>
+    <t>ltblUtilityType</t>
+  </si>
+  <si>
+    <t>varUtilityType</t>
+  </si>
+  <si>
+    <t>Disposition Class</t>
+  </si>
+  <si>
+    <t>ltblDispositionClass</t>
+  </si>
+  <si>
+    <t>varDispositionClass</t>
+  </si>
+  <si>
+    <t>Responsible Division</t>
+  </si>
+  <si>
+    <t>ltblResponsibleDivision</t>
+  </si>
+  <si>
+    <t>varResponsibleDivision</t>
+  </si>
+  <si>
+    <t>Responsible Employee</t>
+  </si>
+  <si>
+    <t>ltblResponsibleEmployee</t>
+  </si>
+  <si>
+    <t>varResponsibleEmployee</t>
+  </si>
+  <si>
+    <t>Domain Class</t>
+  </si>
+  <si>
+    <t>ltblRelateLandToDispositionLandDomainClass</t>
+  </si>
+  <si>
+    <t>Old File Type</t>
+  </si>
+  <si>
+    <t>ltblRelateLandToDispositionLandOldFileType</t>
+  </si>
+  <si>
+    <t>varOldFileType</t>
+  </si>
+  <si>
+    <t>Event Type</t>
+  </si>
+  <si>
+    <t>varEventType</t>
+  </si>
+  <si>
+    <t>Evaluation Recommendation</t>
+  </si>
+  <si>
+    <t>ltblManagementRecommendation</t>
+  </si>
+  <si>
+    <t>varManagementRecommendation</t>
+  </si>
+  <si>
+    <t>Direct Sale</t>
+  </si>
+  <si>
+    <t>varDirectSaleIndicator</t>
+  </si>
+  <si>
+    <t>GLO Land Manager</t>
+  </si>
+  <si>
+    <t>ltblGLOLandManager</t>
+  </si>
+  <si>
+    <t>varGlolandManager</t>
+  </si>
+  <si>
+    <t>ltblPerformanceClass</t>
+  </si>
+  <si>
+    <t>varPerformanceClass</t>
+  </si>
+  <si>
+    <t>Investment Type</t>
+  </si>
+  <si>
+    <t>ltblStrategicClass</t>
+  </si>
+  <si>
+    <t>varStrategicClass</t>
+  </si>
+  <si>
+    <t>Survey Required</t>
+  </si>
+  <si>
+    <t>ltblSurveyRequiredIndicator</t>
+  </si>
+  <si>
+    <t>varSurveyRequiredIndicator</t>
+  </si>
+  <si>
+    <t>Internal Investment Portfolio</t>
+  </si>
+  <si>
+    <t>ltblLandInternalInvestmentPortfolioIndicator</t>
+  </si>
+  <si>
+    <t>varInternalInvestmentPortfolioIndicator</t>
+  </si>
+  <si>
+    <t>Timber Management Plan</t>
+  </si>
+  <si>
+    <t>ltblTimberManagementPlanIndicator</t>
+  </si>
+  <si>
+    <t>varTimberManagementPlanIndicator</t>
+  </si>
+  <si>
+    <t>Uplands Work Area</t>
+  </si>
+  <si>
+    <t>varUplandsWorkArea</t>
+  </si>
+  <si>
+    <t>Inspection Priority</t>
+  </si>
+  <si>
+    <t>ltblInspectionPriority</t>
+  </si>
+  <si>
+    <t>varInspectionPriority</t>
   </si>
   <si>
     <t>username</t>
@@ -705,44 +1035,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -773,7 +1075,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,6 +1098,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -809,9 +1140,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -870,13 +1200,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,55 +1254,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,12 +1278,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -972,13 +1290,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,43 +1332,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,19 +1362,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,6 +1409,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1090,15 +1435,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1127,17 +1463,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1182,44 +1512,44 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1228,7 +1558,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1237,92 +1567,92 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1403,10 +1733,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1757,7 +2084,7 @@
     <col min="4" max="4" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="36" customFormat="1" ht="15" spans="1:4">
+    <row r="1" s="35" customFormat="1" ht="15" spans="1:4">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -1771,11 +2098,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="1" ht="15" spans="1:4">
+    <row r="2" s="36" customFormat="1" ht="15" spans="1:4">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="33" t="s">
@@ -1785,21 +2112,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" s="37" customFormat="1" ht="15" spans="1:4">
+    <row r="3" s="36" customFormat="1" ht="15" spans="1:4">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="37" customFormat="1" ht="15" spans="1:4">
+    <row r="4" s="36" customFormat="1" ht="15" spans="1:4">
       <c r="A4" s="33" t="s">
         <v>11</v>
       </c>
@@ -1814,100 +2141,100 @@
       </c>
     </row>
     <row r="5" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="39" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="15" spans="1:4">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1921,10 +2248,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -1944,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>3</v>
@@ -1952,49 +2279,49 @@
     </row>
     <row r="2" s="28" customFormat="1" ht="27.75" customHeight="1" spans="1:4">
       <c r="A2" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="31" t="s">
+      <c r="D2" s="31" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" s="29" customFormat="1" ht="23.25" customHeight="1" spans="1:4">
       <c r="A3" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="31" t="s">
+    </row>
+    <row r="4" s="2" customFormat="1" ht="21" customHeight="1" spans="1:4">
+      <c r="A4" s="32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="24" customHeight="1" spans="1:4">
-      <c r="A4" s="32" t="s">
+      <c r="B4" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="D4" s="32" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" ht="21" customHeight="1" spans="1:4">
       <c r="A5" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>12</v>
@@ -2008,170 +2335,718 @@
     </row>
     <row r="6" s="29" customFormat="1" ht="20.25" customHeight="1" spans="1:4">
       <c r="A6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="31" t="s">
+      <c r="D6" s="31" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" s="29" customFormat="1" ht="23.25" customHeight="1" spans="1:4">
       <c r="A7" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="31" t="s">
+      <c r="D7" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="31" t="s">
+    </row>
+    <row r="8" ht="21" customHeight="1" spans="1:4">
+      <c r="A8" s="32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" ht="22.5" customHeight="1" spans="1:4">
-      <c r="A8" s="32" t="s">
+      <c r="B8" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="32" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" s="29" customFormat="1" ht="23.25" customHeight="1" spans="1:4">
       <c r="A9" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="31" t="s">
+      <c r="D9" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="31" t="s">
+    </row>
+    <row r="10" s="29" customFormat="1" ht="20" customHeight="1" spans="1:4">
+      <c r="A10" s="31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" s="29" customFormat="1" ht="22.5" customHeight="1" spans="1:4">
-      <c r="A10" s="31" t="s">
+      <c r="B10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="31" t="s">
+    </row>
+    <row r="11" s="29" customFormat="1" ht="22.5" customHeight="1" spans="1:4">
+      <c r="A11" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="B11" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" s="29" customFormat="1" ht="21" customHeight="1" spans="1:4">
-      <c r="A11" s="31" t="s">
+      <c r="D11" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="31" t="s">
+    </row>
+    <row r="12" s="29" customFormat="1" ht="21" customHeight="1" spans="1:4">
+      <c r="A12" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="B12" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" s="29" customFormat="1" ht="23.25" customHeight="1" spans="1:4">
-      <c r="A12" s="33" t="s">
+      <c r="D12" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="31" t="s">
+    </row>
+    <row r="13" s="29" customFormat="1" ht="21" customHeight="1" spans="1:4">
+      <c r="A13" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="B13" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" ht="15" spans="1:4">
-      <c r="A13" s="34" t="s">
+      <c r="D13" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="34" t="s">
+    </row>
+    <row r="14" ht="15" spans="1:4">
+      <c r="A14" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="B14" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" ht="15" spans="1:4">
-      <c r="A14" s="34" t="s">
+      <c r="D14" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="34" t="s">
+    </row>
+    <row r="15" ht="15" spans="1:4">
+      <c r="A15" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="B15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" ht="15" spans="1:4">
-      <c r="A15" s="34" t="s">
+      <c r="D15" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="35" t="s">
+    </row>
+    <row r="16" ht="15" spans="1:4">
+      <c r="A16" s="32" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" ht="15" spans="1:4">
-      <c r="A16" s="34" t="s">
+      <c r="B16" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="34" t="s">
+      <c r="D16" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="34" t="s">
+    </row>
+    <row r="17" ht="15" spans="1:4">
+      <c r="A17" s="32" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" ht="15" spans="1:4">
-      <c r="A17" s="34" t="s">
+      <c r="B17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="34" t="s">
+      <c r="D17" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="34" t="s">
+    </row>
+    <row r="18" ht="15" spans="1:4">
+      <c r="A18" s="32" t="s">
         <v>78</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" ht="15" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" ht="15" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" ht="15" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="34"/>
+      <c r="D31" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" ht="15" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" ht="15" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" ht="15" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" ht="15" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" ht="15" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" ht="15" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" ht="15" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" ht="15" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" ht="15" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" ht="15" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" ht="15" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" ht="15" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" ht="15" spans="1:4">
+      <c r="A44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" ht="30" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" ht="30" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" ht="15" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" ht="15" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" ht="15" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" ht="15" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" ht="15" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" ht="15" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" ht="15" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" ht="30" spans="1:4">
+      <c r="A54" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" ht="30" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" ht="15" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="34"/>
+      <c r="D56" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" ht="15" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2200,63 +3075,63 @@
   <sheetData>
     <row r="1" s="23" customFormat="1" ht="20.25" customHeight="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>189</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" s="24" customFormat="1" ht="15" spans="1:3">
       <c r="A2" s="25" t="s">
-        <v>82</v>
+        <v>192</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>83</v>
+        <v>193</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>84</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" s="24" customFormat="1" ht="16.5" customHeight="1" spans="1:3">
       <c r="A3" s="25" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" s="24" customFormat="1" ht="18.75" customHeight="1" spans="1:3">
       <c r="A4" s="25" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" s="24" customFormat="1" ht="15" spans="1:3">
       <c r="A5" s="25" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C5" s="26"/>
     </row>
     <row r="6" s="24" customFormat="1" ht="15" spans="1:3">
       <c r="A6" s="25" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -2301,10 +3176,10 @@
   <sheetData>
     <row r="1" s="18" customFormat="1" ht="15" spans="1:14">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2313,25 +3188,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>98</v>
+        <v>208</v>
       </c>
       <c r="L1" s="13"/>
       <c r="M1" s="15"/>
@@ -2339,31 +3214,31 @@
     </row>
     <row r="2" ht="15" spans="1:14">
       <c r="A2" s="19" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>103</v>
+        <v>213</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>107</v>
+        <v>217</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -2371,31 +3246,31 @@
     </row>
     <row r="3" ht="28.5" spans="1:14">
       <c r="A3" s="19" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>109</v>
+        <v>219</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>111</v>
+        <v>221</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>116</v>
+        <v>226</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -2403,111 +3278,111 @@
     </row>
     <row r="4" ht="28.5" spans="1:13">
       <c r="A4" s="19" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>118</v>
+        <v>228</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>119</v>
+        <v>229</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
     <row r="5" ht="28.5" spans="1:11">
       <c r="A5" s="19" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>122</v>
+        <v>232</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>123</v>
+        <v>233</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>124</v>
+        <v>234</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>109</v>
+        <v>219</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" ht="28.5" spans="1:11">
       <c r="A6" s="16" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>125</v>
+        <v>235</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>126</v>
+        <v>236</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>116</v>
+        <v>226</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>107</v>
+        <v>217</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>116</v>
+        <v>226</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" ht="28.5" spans="1:13">
       <c r="A7" s="19" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>127</v>
+        <v>237</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>128</v>
+        <v>238</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>129</v>
+        <v>239</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>116</v>
+        <v>226</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
@@ -2547,10 +3422,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:14">
       <c r="A1" s="13" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2559,25 +3434,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>94</v>
+        <v>204</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>96</v>
+        <v>206</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>97</v>
+        <v>207</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>98</v>
+        <v>208</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>25</v>
@@ -2591,78 +3466,78 @@
     </row>
     <row r="2" ht="30" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>227</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>228</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>103</v>
+        <v>213</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>106</v>
+        <v>216</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>124</v>
+        <v>234</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>130</v>
+        <v>240</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>131</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>132</v>
+        <v>242</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>133</v>
+        <v>243</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>222</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>115</v>
+        <v>225</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>114</v>
+        <v>224</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>134</v>
+        <v>244</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>136</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2692,70 +3567,70 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="15" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" ht="60" customHeight="1" spans="1:4">
       <c r="A2" s="10" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>143</v>
+        <v>253</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>144</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" ht="60.75" customHeight="1" spans="1:4">
       <c r="A3" s="10" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>145</v>
+        <v>255</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>146</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" ht="76.5" customHeight="1" spans="1:4">
       <c r="A4" s="10" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>147</v>
+        <v>257</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>146</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" ht="62.25" customHeight="1" spans="1:4">
       <c r="A5" s="10" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>148</v>
+        <v>258</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
-        <v>149</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2791,172 +3666,172 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" ht="21" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" ht="53.25" customHeight="1" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>154</v>
+        <v>264</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>155</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" ht="56.25" customHeight="1" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>156</v>
+        <v>266</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" ht="54" customHeight="1" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>268</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>159</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" ht="52.5" customHeight="1" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>270</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>161</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" ht="55.5" customHeight="1" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>162</v>
+        <v>272</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>163</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" ht="53.25" customHeight="1" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>153</v>
+        <v>263</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>164</v>
+        <v>274</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>165</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" ht="53.25" customHeight="1" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>166</v>
+        <v>276</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>168</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" ht="55.5" customHeight="1" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>169</v>
+        <v>279</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>170</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" ht="51" customHeight="1" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>152</v>
+        <v>262</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>171</v>
+        <v>281</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>172</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2996,114 +3871,114 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>137</v>
+        <v>247</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" ht="38.25" customHeight="1" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>283</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>174</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" ht="45" customHeight="1" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>175</v>
+        <v>285</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>176</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" ht="46.5" customHeight="1" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>287</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>178</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" ht="44.25" customHeight="1" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>179</v>
+        <v>289</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>180</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" ht="45.75" customHeight="1" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>181</v>
+        <v>291</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>182</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" ht="43.5" customHeight="1" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>183</v>
+        <v>293</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>184</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" ht="45" customHeight="1" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>185</v>
+        <v>295</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the location tab
</commit_message>
<xml_diff>
--- a/UI/getdata/TestData.xlsx
+++ b/UI/getdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\UI\getdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C416445-3127-4253-8AF8-C071973A5D2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3E415B-5787-4B57-8710-1593B1060A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="306">
   <si>
     <t>fieldName</t>
   </si>
@@ -152,528 +152,525 @@
     <t>ltblCountyToRRCDistrictNumber</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>varUtilizationClass</t>
+  </si>
+  <si>
+    <t>varUtilizationType</t>
+  </si>
+  <si>
+    <t>varLandCommentClass</t>
+  </si>
+  <si>
+    <t>varMultiTractSaleIndicator</t>
+  </si>
+  <si>
+    <t>varReservationEasementIndicator</t>
+  </si>
+  <si>
+    <t>ltblReservations</t>
+  </si>
+  <si>
+    <t>varReservations</t>
+  </si>
+  <si>
+    <t>varTermsOffered</t>
+  </si>
+  <si>
+    <t>varDirectionFromCountySeat</t>
+  </si>
+  <si>
+    <t>varDeviationFromCountySeat</t>
+  </si>
+  <si>
+    <t>varLandCityName</t>
+  </si>
+  <si>
+    <t>varLegalAccessIndicator</t>
+  </si>
+  <si>
+    <t>varWithinCityIndicator</t>
+  </si>
+  <si>
+    <t>varLandEncumbranceClass</t>
+  </si>
+  <si>
+    <t>varImprovementType</t>
+  </si>
+  <si>
+    <t>varAttributes</t>
+  </si>
+  <si>
+    <t>varImprovementsIndicator</t>
+  </si>
+  <si>
+    <t>varUtilitiesAvailableIndicator</t>
+  </si>
+  <si>
+    <t>varSurroundingUseClass</t>
+  </si>
+  <si>
+    <t>ltblBasefilePrefix</t>
+  </si>
+  <si>
+    <t>varBasefilePrefix</t>
+  </si>
+  <si>
+    <t>ltblBasefileSuffix</t>
+  </si>
+  <si>
+    <t>varBasefileSuffix</t>
+  </si>
+  <si>
+    <t>varAcquisitionClass</t>
+  </si>
+  <si>
+    <t>varAcquisitionMethod</t>
+  </si>
+  <si>
+    <t>varExcessStatus</t>
+  </si>
+  <si>
+    <t>varWaterBody</t>
+  </si>
+  <si>
+    <t>varLandType</t>
+  </si>
+  <si>
+    <t>varLandOwnershipClass</t>
+  </si>
+  <si>
+    <t>varLandGeographicClass</t>
+  </si>
+  <si>
+    <t>varLandDomainClass</t>
+  </si>
+  <si>
+    <t>varLandStatus</t>
+  </si>
+  <si>
+    <t>ltblAppraisalSource</t>
+  </si>
+  <si>
+    <t>varAppraisalSource</t>
+  </si>
+  <si>
+    <t>varEstimatedValueMethod</t>
+  </si>
+  <si>
+    <t>varUtilityType</t>
+  </si>
+  <si>
+    <t>varDispositionClass</t>
+  </si>
+  <si>
+    <t>varResponsibleDivision</t>
+  </si>
+  <si>
+    <t>varResponsibleEmployee</t>
+  </si>
+  <si>
+    <t>varOldFileType</t>
+  </si>
+  <si>
+    <t>varEventType</t>
+  </si>
+  <si>
+    <t>varManagementRecommendation</t>
+  </si>
+  <si>
+    <t>varGlolandManager</t>
+  </si>
+  <si>
+    <t>varPerformanceClass</t>
+  </si>
+  <si>
+    <t>varStrategicClass</t>
+  </si>
+  <si>
+    <t>varSurveyRequiredIndicator</t>
+  </si>
+  <si>
+    <t>varInternalInvestmentPortfolioIndicator</t>
+  </si>
+  <si>
+    <t>varTimberManagementPlanIndicator</t>
+  </si>
+  <si>
+    <t>varInspectionPriority</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>yan.liu@an-chen.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lychan@2012 </t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>1925719012@qq.com</t>
+  </si>
+  <si>
+    <t>Abc1234%</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>tangjiu2020@163.com</t>
+  </si>
+  <si>
+    <t>Read Only</t>
+  </si>
+  <si>
+    <t>elena022@163.com</t>
+  </si>
+  <si>
+    <t>elena011@163.com</t>
+  </si>
+  <si>
+    <t>entityType</t>
+  </si>
+  <si>
+    <t>entityClass</t>
+  </si>
+  <si>
+    <t>typeOfBusiness</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>type1</t>
+  </si>
+  <si>
+    <t>type2</t>
+  </si>
+  <si>
+    <t>type3</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Sr.</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>CPA</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Sole Proprietor</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>D.D.S.</t>
+  </si>
+  <si>
+    <t>Clerk</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Limited Liability Company</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Trust/Estate</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>State Tax ID</t>
+  </si>
+  <si>
+    <t>Rev.</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>Mailing</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Internal GLO ID</t>
+  </si>
+  <si>
+    <t>first_menu</t>
+  </si>
+  <si>
+    <t>second_menu</t>
+  </si>
+  <si>
+    <t>third_menu</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>customers</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>ALAMO CRM Checklist</t>
+  </si>
+  <si>
+    <t>http://talon:8080/alamo/links/Production/ALAMO%20CRM%20Checklist.pdf</t>
+  </si>
+  <si>
+    <t>Blanket Authorization Royalty Reports Affidavit</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Testing/Public/ApplicationReports/ALAMO/Blanket+Authorization+Royalty+Reports+Affidavit</t>
+  </si>
+  <si>
+    <t>MIP Customer Activity</t>
+  </si>
+  <si>
+    <t>CRM Style Guide</t>
+  </si>
+  <si>
+    <t>https://iglo.glo.state.tx.us/ssf/a/c/p_name/ss_forum/p_action/1/action/view_permalink/entityType/folderEntry/entryId/56873/vibeonprem_url/1</t>
+  </si>
+  <si>
+    <t>four_menu</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>Inventory Update Forms</t>
+  </si>
+  <si>
+    <t>PSF</t>
+  </si>
+  <si>
+    <t>Acquisitions</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Acquisitions%20master-15-2-19.xls</t>
+  </si>
+  <si>
+    <t>Additions</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Additions.xls</t>
+  </si>
+  <si>
+    <t>Dispositions</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Dispositions2014.xls</t>
+  </si>
+  <si>
+    <t>Appraisal</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AppraisalUpdate.xls</t>
+  </si>
+  <si>
+    <t>Adjustment - Inventory</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AdjustmentsToCurrentInv.xls</t>
+  </si>
+  <si>
+    <t>Adjustment - Dispositions</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AdjustmentsToDispositions.xls</t>
+  </si>
+  <si>
+    <t>Vacancy</t>
+  </si>
+  <si>
+    <t>Disposition</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/vacancy/InventoryUpdateForm-Dispositions.xls</t>
+  </si>
+  <si>
+    <t>Excess Acreage</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/excess_acreage/InventoryUpdateForm-ExcessAcreage.xls</t>
+  </si>
+  <si>
+    <t>Tax Foreclosure</t>
+  </si>
+  <si>
+    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/tax_foreclosure/InventoryUpdateForm-Dispositions.xls</t>
+  </si>
+  <si>
+    <t>AM Acquisition Report</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/AM+Acquisition+Report</t>
+  </si>
+  <si>
+    <t>AM Disposition Report</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/AM+Disposition+Report</t>
+  </si>
+  <si>
+    <t>PSF Evaluation Report</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_Evaluations</t>
+  </si>
+  <si>
+    <t>PSF Land Available For Direct Sale</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_Direct+_Sale_List</t>
+  </si>
+  <si>
+    <t>PSF Land Quarterly Report</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF+Land+Quarterly+Report</t>
+  </si>
+  <si>
+    <t>PSF SBS Current List</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_SBS_Current_Sale_List</t>
+  </si>
+  <si>
+    <t>State Street</t>
+  </si>
+  <si>
+    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/State+Street+Property+Report</t>
+  </si>
+  <si>
+    <t>ltblEventType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>varDirectSaleIndicator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltblDirectSaleIndicator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>varMineralsSoldIndicator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltblMineralsSoldIndicator</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>varRelateLandToLandRelateClass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltblRelateLandToLandRelateClass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltblAcquisitionClass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltblAcquisitionMethod</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>acquisitionClass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>acquisitionMethod</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>varCountyName</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>varUtilizationClass</t>
-  </si>
-  <si>
-    <t>varUtilizationType</t>
-  </si>
-  <si>
-    <t>varLandCommentClass</t>
-  </si>
-  <si>
-    <t>varMultiTractSaleIndicator</t>
-  </si>
-  <si>
-    <t>varReservationEasementIndicator</t>
-  </si>
-  <si>
-    <t>ltblReservations</t>
-  </si>
-  <si>
-    <t>varReservations</t>
-  </si>
-  <si>
-    <t>varTermsOffered</t>
-  </si>
-  <si>
-    <t>varDirectionFromCountySeat</t>
-  </si>
-  <si>
-    <t>varDeviationFromCountySeat</t>
-  </si>
-  <si>
-    <t>varLandCityName</t>
-  </si>
-  <si>
-    <t>varLegalAccessIndicator</t>
-  </si>
-  <si>
-    <t>varWithinCityIndicator</t>
-  </si>
-  <si>
-    <t>varLandEncumbranceClass</t>
-  </si>
-  <si>
-    <t>varImprovementType</t>
-  </si>
-  <si>
-    <t>varAttributes</t>
-  </si>
-  <si>
-    <t>varImprovementsIndicator</t>
-  </si>
-  <si>
-    <t>varUtilitiesAvailableIndicator</t>
-  </si>
-  <si>
-    <t>varSurroundingUseClass</t>
-  </si>
-  <si>
-    <t>ltblBasefilePrefix</t>
-  </si>
-  <si>
-    <t>varBasefilePrefix</t>
-  </si>
-  <si>
-    <t>ltblBasefileSuffix</t>
-  </si>
-  <si>
-    <t>varBasefileSuffix</t>
-  </si>
-  <si>
-    <t>varAcquisitionClass</t>
-  </si>
-  <si>
-    <t>varAcquisitionMethod</t>
-  </si>
-  <si>
-    <t>varExcessStatus</t>
-  </si>
-  <si>
-    <t>varWaterBody</t>
-  </si>
-  <si>
-    <t>varLandType</t>
-  </si>
-  <si>
-    <t>varLandOwnershipClass</t>
-  </si>
-  <si>
-    <t>varLandGeographicClass</t>
-  </si>
-  <si>
-    <t>varLandDomainClass</t>
-  </si>
-  <si>
-    <t>varLandStatus</t>
-  </si>
-  <si>
-    <t>ltblAppraisalSource</t>
-  </si>
-  <si>
-    <t>varAppraisalSource</t>
-  </si>
-  <si>
-    <t>varEstimatedValueMethod</t>
-  </si>
-  <si>
-    <t>varUtilityType</t>
-  </si>
-  <si>
-    <t>varDispositionClass</t>
-  </si>
-  <si>
-    <t>varResponsibleDivision</t>
-  </si>
-  <si>
-    <t>varResponsibleEmployee</t>
-  </si>
-  <si>
-    <t>varOldFileType</t>
-  </si>
-  <si>
-    <t>varEventType</t>
-  </si>
-  <si>
-    <t>varManagementRecommendation</t>
-  </si>
-  <si>
-    <t>varGlolandManager</t>
-  </si>
-  <si>
-    <t>varPerformanceClass</t>
-  </si>
-  <si>
-    <t>varStrategicClass</t>
-  </si>
-  <si>
-    <t>varSurveyRequiredIndicator</t>
-  </si>
-  <si>
-    <t>varInternalInvestmentPortfolioIndicator</t>
-  </si>
-  <si>
-    <t>varTimberManagementPlanIndicator</t>
-  </si>
-  <si>
-    <t>varInspectionPriority</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>yan.liu@an-chen.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lychan@2012 </t>
-  </si>
-  <si>
-    <t>Master</t>
-  </si>
-  <si>
-    <t>1925719012@qq.com</t>
-  </si>
-  <si>
-    <t>Abc1234%</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>tangjiu2020@163.com</t>
-  </si>
-  <si>
-    <t>Read Only</t>
-  </si>
-  <si>
-    <t>elena022@163.com</t>
-  </si>
-  <si>
-    <t>elena011@163.com</t>
-  </si>
-  <si>
-    <t>entityType</t>
-  </si>
-  <si>
-    <t>entityClass</t>
-  </si>
-  <si>
-    <t>typeOfBusiness</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>type1</t>
-  </si>
-  <si>
-    <t>type2</t>
-  </si>
-  <si>
-    <t>type3</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>Miss</t>
-  </si>
-  <si>
-    <t>Sr.</t>
-  </si>
-  <si>
-    <t>Agent</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>County</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>CPA</t>
-  </si>
-  <si>
-    <t>Personal</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>Sole Proprietor</t>
-  </si>
-  <si>
-    <t>Dr.</t>
-  </si>
-  <si>
-    <t>D.D.S.</t>
-  </si>
-  <si>
-    <t>Clerk</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Limited Liability Company</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>Consultant</t>
-  </si>
-  <si>
-    <t>Household</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
-    <t>Trust/Estate</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>Analyst</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>State Tax ID</t>
-  </si>
-  <si>
-    <t>Rev.</t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
-    <t>Mailing</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Internal GLO ID</t>
-  </si>
-  <si>
-    <t>first_menu</t>
-  </si>
-  <si>
-    <t>second_menu</t>
-  </si>
-  <si>
-    <t>third_menu</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>customers</t>
-  </si>
-  <si>
-    <t>Reports</t>
-  </si>
-  <si>
-    <t>ALAMO CRM Checklist</t>
-  </si>
-  <si>
-    <t>http://talon:8080/alamo/links/Production/ALAMO%20CRM%20Checklist.pdf</t>
-  </si>
-  <si>
-    <t>Blanket Authorization Royalty Reports Affidavit</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Testing/Public/ApplicationReports/ALAMO/Blanket+Authorization+Royalty+Reports+Affidavit</t>
-  </si>
-  <si>
-    <t>MIP Customer Activity</t>
-  </si>
-  <si>
-    <t>CRM Style Guide</t>
-  </si>
-  <si>
-    <t>https://iglo.glo.state.tx.us/ssf/a/c/p_name/ss_forum/p_action/1/action/view_permalink/entityType/folderEntry/entryId/56873/vibeonprem_url/1</t>
-  </si>
-  <si>
-    <t>four_menu</t>
-  </si>
-  <si>
-    <t>land</t>
-  </si>
-  <si>
-    <t>Inventory Update Forms</t>
-  </si>
-  <si>
-    <t>PSF</t>
-  </si>
-  <si>
-    <t>Acquisitions</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Acquisitions%20master-15-2-19.xls</t>
-  </si>
-  <si>
-    <t>Additions</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Additions.xls</t>
-  </si>
-  <si>
-    <t>Dispositions</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-Dispositions2014.xls</t>
-  </si>
-  <si>
-    <t>Appraisal</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AppraisalUpdate.xls</t>
-  </si>
-  <si>
-    <t>Adjustment - Inventory</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AdjustmentsToCurrentInv.xls</t>
-  </si>
-  <si>
-    <t>Adjustment - Dispositions</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/psf/InventoryUpdateForm-AdjustmentsToDispositions.xls</t>
-  </si>
-  <si>
-    <t>Vacancy</t>
-  </si>
-  <si>
-    <t>Disposition</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/vacancy/InventoryUpdateForm-Dispositions.xls</t>
-  </si>
-  <si>
-    <t>Excess Acreage</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/excess_acreage/InventoryUpdateForm-ExcessAcreage.xls</t>
-  </si>
-  <si>
-    <t>Tax Foreclosure</t>
-  </si>
-  <si>
-    <t>https://rr-alamo-test.azureedge.net/Inventory_update_forms/tax_foreclosure/InventoryUpdateForm-Dispositions.xls</t>
-  </si>
-  <si>
-    <t>AM Acquisition Report</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/AM+Acquisition+Report</t>
-  </si>
-  <si>
-    <t>AM Disposition Report</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/AM+Disposition+Report</t>
-  </si>
-  <si>
-    <t>PSF Evaluation Report</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_Evaluations</t>
-  </si>
-  <si>
-    <t>PSF Land Available For Direct Sale</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_Direct+_Sale_List</t>
-  </si>
-  <si>
-    <t>PSF Land Quarterly Report</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF+Land+Quarterly+Report</t>
-  </si>
-  <si>
-    <t>PSF SBS Current List</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/PSF_SBS_Current_Sale_List</t>
-  </si>
-  <si>
-    <t>State Street</t>
-  </si>
-  <si>
-    <t>http://gloreports/ReportServer/Pages/ReportViewer.aspx?/Production/Public/ApplicationReports/ALAMO/State+Street+Property+Report</t>
-  </si>
-  <si>
-    <t>ltblEventType</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>varDirectSaleIndicator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltblDirectSaleIndicator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>varMineralsSoldIndicator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltblMineralsSoldIndicator</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>varRelateLandToLandRelateClass</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltblRelateLandToLandRelateClass</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltblAcquisitionClass</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ltblAcquisitionMethod</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>acquisitionClass</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>acquisitionMethod</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>varCountyName</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1046,6 +1043,14 @@
   </si>
   <si>
     <t>performanceClass</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>vewLookupCounty</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>varCounty</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1791,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1854,15 +1859,15 @@
         <v>12</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>40</v>
+        <v>304</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>41</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>12</v>
@@ -1876,329 +1881,329 @@
     </row>
     <row r="6" spans="1:4" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>278</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>279</v>
-      </c>
       <c r="D10" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="42" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>48</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B20" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>12</v>
@@ -2207,399 +2212,399 @@
         <v>40</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B30" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B32" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B33" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B34" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B35" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B36" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B38" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B40" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B47" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B48" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B49" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B53" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B54" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B55" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B56" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B57" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2627,63 +2632,63 @@
   <sheetData>
     <row r="1" spans="1:3" s="23" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -2727,10 +2732,10 @@
   <sheetData>
     <row r="1" spans="1:14" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2739,25 +2744,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="L1" s="13"/>
       <c r="M1" s="15"/>
@@ -2765,31 +2770,31 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -2797,31 +2802,31 @@
     </row>
     <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -2829,111 +2834,111 @@
     </row>
     <row r="4" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="G4" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>134</v>
-      </c>
       <c r="I4" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>122</v>
-      </c>
       <c r="I5" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>139</v>
-      </c>
       <c r="H6" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>142</v>
-      </c>
       <c r="H7" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="21" t="s">
         <v>118</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>119</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
@@ -2972,10 +2977,10 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2984,25 +2989,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>25</v>
@@ -3016,78 +3021,78 @@
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>119</v>
-      </c>
       <c r="K2" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="N2" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="L3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>148</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3116,70 +3121,70 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>156</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="C3" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>158</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="C4" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3214,172 +3219,172 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C10" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3418,114 +3423,114 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cases for characteristic tab
</commit_message>
<xml_diff>
--- a/UI/getdata/TestData.xlsx
+++ b/UI/getdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation\UI\getdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3E415B-5787-4B57-8710-1593B1060A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335E9B63-ABF7-4FB0-9CBC-066F565C3E58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>varImprovementType</t>
   </si>
   <si>
-    <t>varAttributes</t>
-  </si>
-  <si>
     <t>varImprovementsIndicator</t>
   </si>
   <si>
@@ -1051,6 +1048,10 @@
   </si>
   <si>
     <t>varCounty</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>varDispositionAttribute</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1796,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1859,10 +1860,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>304</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,13 +1882,13 @@
     </row>
     <row r="6" spans="1:4" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>42</v>
@@ -1895,13 +1896,13 @@
     </row>
     <row r="7" spans="1:4" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>43</v>
@@ -1909,13 +1910,13 @@
     </row>
     <row r="8" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>44</v>
@@ -1923,13 +1924,13 @@
     </row>
     <row r="9" spans="1:4" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D9" s="40" t="s">
         <v>45</v>
@@ -1937,27 +1938,27 @@
     </row>
     <row r="10" spans="1:4" s="42" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>278</v>
-      </c>
       <c r="D10" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="42" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>46</v>
@@ -1965,7 +1966,7 @@
     </row>
     <row r="12" spans="1:4" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>12</v>
@@ -1979,13 +1980,13 @@
     </row>
     <row r="13" spans="1:4" s="42" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>49</v>
@@ -1993,13 +1994,13 @@
     </row>
     <row r="14" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B14" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>50</v>
@@ -2007,13 +2008,13 @@
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>51</v>
@@ -2021,13 +2022,13 @@
     </row>
     <row r="16" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>52</v>
@@ -2035,13 +2036,13 @@
     </row>
     <row r="17" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>53</v>
@@ -2049,13 +2050,13 @@
     </row>
     <row r="18" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>54</v>
@@ -2063,13 +2064,13 @@
     </row>
     <row r="19" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B19" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>55</v>
@@ -2077,13 +2078,13 @@
     </row>
     <row r="20" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>56</v>
@@ -2091,119 +2092,119 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B21" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>57</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B24" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B25" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B26" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29" s="40" t="s">
         <v>12</v>
@@ -2212,399 +2213,399 @@
         <v>40</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B30" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B33" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B34" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B35" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B36" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B37" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B38" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B39" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B40" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B46" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B47" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B48" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B49" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B53" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B54" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B55" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B56" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B57" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2632,63 +2633,63 @@
   <sheetData>
     <row r="1" spans="1:3" s="23" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="24" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" s="24" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -2732,10 +2733,10 @@
   <sheetData>
     <row r="1" spans="1:14" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2744,25 +2745,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="L1" s="13"/>
       <c r="M1" s="15"/>
@@ -2770,31 +2771,31 @@
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="G2" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="19" t="s">
         <v>118</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>119</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
@@ -2802,31 +2803,31 @@
     </row>
     <row r="3" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="E3" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22"/>
@@ -2834,111 +2835,111 @@
     </row>
     <row r="4" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="G4" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="I4" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>121</v>
-      </c>
       <c r="I5" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>138</v>
-      </c>
       <c r="H6" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="G7" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>141</v>
-      </c>
       <c r="H7" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>118</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
@@ -2977,10 +2978,10 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>4</v>
@@ -2989,25 +2990,25 @@
         <v>8</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>25</v>
@@ -3021,78 +3022,78 @@
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>118</v>
-      </c>
       <c r="K2" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M2" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="G3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="L3" s="17" t="s">
+      <c r="M3" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="N3" s="16" t="s">
         <v>147</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3121,70 +3122,70 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="C3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>154</v>
-      </c>
       <c r="C4" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3219,172 +3220,172 @@
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="D7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C8" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3423,114 +3424,114 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>